<commit_message>
further tests for discharge norms
</commit_message>
<xml_diff>
--- a/sapphire_backend/metrics/tests/data/decadal_norm_example.xlsx
+++ b/sapphire_backend/metrics/tests/data/decadal_norm_example.xlsx
@@ -237,10 +237,10 @@
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK9" activeCellId="0" sqref="AK9"/>
+      <selection pane="topLeft" activeCell="AH19" activeCellId="0" sqref="AH19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -360,148 +360,112 @@
         <v>37</v>
       </c>
       <c r="B2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
+      <c r="K2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>10</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>8</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>2</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>2</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>5</v>
-      </c>
       <c r="L2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="O2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="P2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="R2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="S2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="T2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="U2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="V2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="W2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="X2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="Y2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="Z2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="AA2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="AB2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="AC2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="AD2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="AE2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="AF2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="AG2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="AH2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="AI2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="AJ2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="AK2" s="1" t="n">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1, 10)</f>
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>